<commit_message>
update 03_compile_big to make annual and aggreagte journal count plots
</commit_message>
<xml_diff>
--- a/results/missing_software.xlsx
+++ b/results/missing_software.xlsx
@@ -12,29 +12,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>paper</t>
   </si>
   <si>
+    <t>101 hanasoge aa14345-10.pdf</t>
+  </si>
+  <si>
+    <t>107 heister 2010-eccomas.pdf</t>
+  </si>
+  <si>
     <t>108 heister chp%3A10.1007%2F978-3-642-15646-5_13.pdf</t>
   </si>
   <si>
+    <t>13 Geology-2013-Ballmer-G33804.1.pdf</t>
+  </si>
+  <si>
     <t>130 van summeren 2041-8205_736_1_L15.pdf</t>
   </si>
   <si>
     <t>131 kaneko 1-s2.0-S0040195110002684-main.pdf</t>
   </si>
   <si>
+    <t>132 Geophys. J. Int.-2014-Kaneko-gji-ggu030.pdf</t>
+  </si>
+  <si>
     <t>134 key nature11932.pdf</t>
   </si>
   <si>
-    <t>139 kom 1-s2.0-S0041624X1100076X-main.pdf</t>
+    <t>14 Ballmer ggge20662.pdf</t>
   </si>
   <si>
     <t>143 kreiss 110832847.pdf</t>
   </si>
   <si>
+    <t>147 Geophys. J. Int.-2015-Lahivaara-1662-75.pdf</t>
+  </si>
+  <si>
     <t>148 lahivaara 0266-5611_30_1_015003.pdf</t>
   </si>
   <si>
@@ -44,12 +59,27 @@
     <t>16 Barbot_et_al-2010-Geophysical_Journal_International.pdf</t>
   </si>
   <si>
+    <t>164 ma Xiao_Ma.pdf</t>
+  </si>
+  <si>
     <t>168 manea Geology-2012-Manea-35-8.pdf</t>
   </si>
   <si>
+    <t>17 Barbot_et_al-2010-Geophysical_Journal_International (1).pdf</t>
+  </si>
+  <si>
     <t>18 Barriere dbfe70dce0b8f0586cd083fe58cad33b5887f39483ffaa7c18a655e0f8b250f3.pdf</t>
   </si>
   <si>
+    <t>183 michea 2c274b5da1f640f282336a91b4d159a812d792d17d8ffb62b1ebb9fc2bc78526.pdf</t>
+  </si>
+  <si>
+    <t>184 michel 06236135.pdf</t>
+  </si>
+  <si>
+    <t>189 motoki ggge20669.pdf</t>
+  </si>
+  <si>
     <t>191 Natarov_et_al-2012-Geophysical_Journal_International.pdf</t>
   </si>
   <si>
@@ -59,37 +89,31 @@
     <t>203 ozgun 2621.full.pdf</t>
   </si>
   <si>
+    <t>207 quere jgrb50102.pdf</t>
+  </si>
+  <si>
     <t>210 rappapport 0004-637X_752_1_1.pdf</t>
   </si>
   <si>
-    <t>214 Geophys. J. Int.-2014-Retailleau-1030-42.pdf</t>
-  </si>
-  <si>
-    <t>215 retailleau adgeo-40-27-2015.pdf</t>
-  </si>
-  <si>
-    <t>216 reay ngeo825.pdf</t>
-  </si>
-  <si>
     <t>217 Geology-2012-Rey-e280.pdf</t>
   </si>
   <si>
-    <t>218s rey 2011124.pdf</t>
-  </si>
-  <si>
     <t>219 Lithosphere-2010-Rey-328-32.pdf</t>
   </si>
   <si>
-    <t>219s rey 2010241.pdf</t>
+    <t>223 Geophys. J. Int.-2013-Ristau-gji-ggt222.pdf</t>
+  </si>
+  <si>
+    <t>226 rollins art%3A10.1007%2Fs00024-014-1005-6.pdf</t>
+  </si>
+  <si>
+    <t>227 rousset jgrb17375.pdf</t>
   </si>
   <si>
     <t>230 savage 1241.full.pdf</t>
   </si>
   <si>
-    <t>241 sjogreen art%3A10.1007%2Fs10915-011-9531-1.pdf</t>
-  </si>
-  <si>
-    <t>254 sun ggge20185.pdf</t>
+    <t>25 bianco jgrb16872.pdf</t>
   </si>
   <si>
     <t>259 thebaud 1-s2.0-S0301926812000769-main.pdf</t>
@@ -110,10 +134,7 @@
     <t>277 vansumm ggge2119.pdf</t>
   </si>
   <si>
-    <t>294 Yuan 1-s2.0-S0012821X13002768-main.pdf</t>
-  </si>
-  <si>
-    <t>295 yuan jgrb50622.pdf</t>
+    <t>278 vansumm jgre20077.pdf</t>
   </si>
   <si>
     <t>30 Boue Geophys. J. Int.-2013-Bouee-844-8.pdf</t>
@@ -134,19 +155,22 @@
     <t>36 ebru j.1365-246X.2011.04970.x.pdf</t>
   </si>
   <si>
+    <t>37 Bruhat.pdf</t>
+  </si>
+  <si>
     <t>51 conrad Geological Society of America Bulletin-2013-Conrad-1027-52.pdf</t>
   </si>
   <si>
     <t>53 conrad nature12203.pdf</t>
   </si>
   <si>
-    <t>6 Appelo 09077223x.pdf</t>
-  </si>
-  <si>
-    <t>65 debaille 1-s2.0-S0012821X13001982-main.pdf</t>
-  </si>
-  <si>
-    <t>81 favretto art%3A10.1007%2Fs11589-014-0061-4.pdf</t>
+    <t>7 arredondo 1-s2.0-S0031920112000349-main.pdf</t>
+  </si>
+  <si>
+    <t>73 drilleau Dupros_parco_2010_ref6125.pdf</t>
+  </si>
+  <si>
+    <t>74 Elkinsannurev-earth-042711-105503 (1).pdf</t>
   </si>
   <si>
     <t>85 Geology-2011-Flament-1159-62.pdf</t>
@@ -430,6 +454,46 @@
         <v>45</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>